<commit_message>
complete valemount data entry
</commit_message>
<xml_diff>
--- a/data-raw/Valemount_Site_data_raw.xlsx
+++ b/data-raw/Valemount_Site_data_raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hgriesba\Documents\Git\larch-dendro-2020\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F44AC3-1ACC-4007-BAC8-CD3C1BB5238A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F1E281-B574-4F7C-9A5A-75671285238D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="40">
   <si>
     <t>Opening</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>160_D23</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>DSG</t>
+  </si>
+  <si>
+    <t>Bl</t>
   </si>
 </sst>
 </file>
@@ -975,7 +984,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1512,11 +1521,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M95"/>
+  <dimension ref="A1:M175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G175" sqref="G175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3547,7 +3556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>36</v>
       </c>
@@ -3570,7 +3579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -3593,7 +3602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>36</v>
       </c>
@@ -3616,7 +3625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>36</v>
       </c>
@@ -3639,7 +3648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>36</v>
       </c>
@@ -3662,7 +3671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>36</v>
       </c>
@@ -3685,7 +3694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>36</v>
       </c>
@@ -3708,7 +3717,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>36</v>
       </c>
@@ -3731,7 +3740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -3754,7 +3763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>36</v>
       </c>
@@ -3777,7 +3786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>36</v>
       </c>
@@ -3800,7 +3809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>36</v>
       </c>
@@ -3823,7 +3832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>36</v>
       </c>
@@ -3846,7 +3855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -3869,7 +3878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>36</v>
       </c>
@@ -3890,6 +3899,1945 @@
       </c>
       <c r="G95">
         <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>36</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>28</v>
+      </c>
+      <c r="E96">
+        <v>11.3</v>
+      </c>
+      <c r="F96">
+        <v>7.6</v>
+      </c>
+      <c r="G96">
+        <v>2</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>36</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97" t="s">
+        <v>27</v>
+      </c>
+      <c r="E97">
+        <v>12.9</v>
+      </c>
+      <c r="F97">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G97">
+        <v>2</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>36</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="C98">
+        <v>3</v>
+      </c>
+      <c r="D98" t="s">
+        <v>28</v>
+      </c>
+      <c r="E98">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F98">
+        <v>8.1</v>
+      </c>
+      <c r="G98">
+        <v>2</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>36</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99">
+        <v>4</v>
+      </c>
+      <c r="D99" t="s">
+        <v>27</v>
+      </c>
+      <c r="E99">
+        <v>11.8</v>
+      </c>
+      <c r="F99">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>36</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100">
+        <v>5</v>
+      </c>
+      <c r="D100" t="s">
+        <v>28</v>
+      </c>
+      <c r="E100">
+        <v>10.5</v>
+      </c>
+      <c r="F100">
+        <v>8.1</v>
+      </c>
+      <c r="G100">
+        <v>2</v>
+      </c>
+      <c r="H100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>36</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+      <c r="C101">
+        <v>6</v>
+      </c>
+      <c r="D101" t="s">
+        <v>28</v>
+      </c>
+      <c r="E101">
+        <v>8.4</v>
+      </c>
+      <c r="F101">
+        <v>7.8</v>
+      </c>
+      <c r="G101">
+        <v>2</v>
+      </c>
+      <c r="H101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>36</v>
+      </c>
+      <c r="B102">
+        <v>2</v>
+      </c>
+      <c r="C102">
+        <v>7</v>
+      </c>
+      <c r="D102" t="s">
+        <v>28</v>
+      </c>
+      <c r="E102">
+        <v>5</v>
+      </c>
+      <c r="F102">
+        <v>6.4</v>
+      </c>
+      <c r="G102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>36</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103">
+        <v>8</v>
+      </c>
+      <c r="D103" t="s">
+        <v>28</v>
+      </c>
+      <c r="E103">
+        <v>4.3</v>
+      </c>
+      <c r="F103">
+        <v>6.3</v>
+      </c>
+      <c r="G103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>36</v>
+      </c>
+      <c r="B104">
+        <v>2</v>
+      </c>
+      <c r="C104">
+        <v>9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>28</v>
+      </c>
+      <c r="E104">
+        <v>5.6</v>
+      </c>
+      <c r="F104">
+        <v>6.6</v>
+      </c>
+      <c r="G104">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>36</v>
+      </c>
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="C105">
+        <v>10</v>
+      </c>
+      <c r="D105" t="s">
+        <v>27</v>
+      </c>
+      <c r="E105">
+        <v>6.9</v>
+      </c>
+      <c r="F105">
+        <v>6.9</v>
+      </c>
+      <c r="G105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>36</v>
+      </c>
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="C106">
+        <v>11</v>
+      </c>
+      <c r="D106" t="s">
+        <v>28</v>
+      </c>
+      <c r="E106">
+        <v>7.6</v>
+      </c>
+      <c r="F106">
+        <v>6.8</v>
+      </c>
+      <c r="G106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>36</v>
+      </c>
+      <c r="B107">
+        <v>2</v>
+      </c>
+      <c r="C107">
+        <v>12</v>
+      </c>
+      <c r="D107" t="s">
+        <v>28</v>
+      </c>
+      <c r="E107">
+        <v>7</v>
+      </c>
+      <c r="F107">
+        <v>6.9</v>
+      </c>
+      <c r="G107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>36</v>
+      </c>
+      <c r="B108">
+        <v>2</v>
+      </c>
+      <c r="C108">
+        <v>13</v>
+      </c>
+      <c r="D108" t="s">
+        <v>28</v>
+      </c>
+      <c r="E108">
+        <v>5.8</v>
+      </c>
+      <c r="F108">
+        <v>5.4</v>
+      </c>
+      <c r="G108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>36</v>
+      </c>
+      <c r="B109">
+        <v>2</v>
+      </c>
+      <c r="C109">
+        <v>14</v>
+      </c>
+      <c r="D109" t="s">
+        <v>28</v>
+      </c>
+      <c r="E109">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F109">
+        <v>7.1</v>
+      </c>
+      <c r="G109">
+        <v>2</v>
+      </c>
+      <c r="H109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>36</v>
+      </c>
+      <c r="B110">
+        <v>2</v>
+      </c>
+      <c r="C110">
+        <v>15</v>
+      </c>
+      <c r="D110" t="s">
+        <v>28</v>
+      </c>
+      <c r="E110">
+        <v>5.4</v>
+      </c>
+      <c r="F110">
+        <v>6.8</v>
+      </c>
+      <c r="G110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>36</v>
+      </c>
+      <c r="B111">
+        <v>2</v>
+      </c>
+      <c r="C111">
+        <v>16</v>
+      </c>
+      <c r="D111" t="s">
+        <v>33</v>
+      </c>
+      <c r="E111">
+        <v>5</v>
+      </c>
+      <c r="F111">
+        <v>4.5</v>
+      </c>
+      <c r="G111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>36</v>
+      </c>
+      <c r="B112">
+        <v>2</v>
+      </c>
+      <c r="C112">
+        <v>17</v>
+      </c>
+      <c r="D112" t="s">
+        <v>27</v>
+      </c>
+      <c r="E112">
+        <v>5.4</v>
+      </c>
+      <c r="F112">
+        <v>6.1</v>
+      </c>
+      <c r="G112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>36</v>
+      </c>
+      <c r="B113">
+        <v>2</v>
+      </c>
+      <c r="C113">
+        <v>18</v>
+      </c>
+      <c r="D113" t="s">
+        <v>27</v>
+      </c>
+      <c r="E113">
+        <v>7.5</v>
+      </c>
+      <c r="F113">
+        <v>7.2</v>
+      </c>
+      <c r="G113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>36</v>
+      </c>
+      <c r="B114">
+        <v>2</v>
+      </c>
+      <c r="C114">
+        <v>19</v>
+      </c>
+      <c r="D114" t="s">
+        <v>28</v>
+      </c>
+      <c r="E114">
+        <v>6.7</v>
+      </c>
+      <c r="F114">
+        <v>6.9</v>
+      </c>
+      <c r="G114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>36</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+      <c r="C115">
+        <v>20</v>
+      </c>
+      <c r="D115" t="s">
+        <v>33</v>
+      </c>
+      <c r="E115">
+        <v>7</v>
+      </c>
+      <c r="F115">
+        <v>6.4</v>
+      </c>
+      <c r="G115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>36</v>
+      </c>
+      <c r="B116">
+        <v>3</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="D116" t="s">
+        <v>28</v>
+      </c>
+      <c r="E116">
+        <v>10.9</v>
+      </c>
+      <c r="F116">
+        <v>8.5</v>
+      </c>
+      <c r="G116">
+        <v>2</v>
+      </c>
+      <c r="H116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>36</v>
+      </c>
+      <c r="B117">
+        <v>3</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117" t="s">
+        <v>28</v>
+      </c>
+      <c r="E117">
+        <v>8</v>
+      </c>
+      <c r="F117">
+        <v>7.7</v>
+      </c>
+      <c r="G117">
+        <v>2</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>36</v>
+      </c>
+      <c r="B118">
+        <v>3</v>
+      </c>
+      <c r="C118">
+        <v>3</v>
+      </c>
+      <c r="D118" t="s">
+        <v>27</v>
+      </c>
+      <c r="E118">
+        <v>10.1</v>
+      </c>
+      <c r="F118">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G118">
+        <v>2</v>
+      </c>
+      <c r="H118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>36</v>
+      </c>
+      <c r="B119">
+        <v>3</v>
+      </c>
+      <c r="C119">
+        <v>4</v>
+      </c>
+      <c r="D119" t="s">
+        <v>28</v>
+      </c>
+      <c r="E119">
+        <v>10.4</v>
+      </c>
+      <c r="F119">
+        <v>7.3</v>
+      </c>
+      <c r="G119">
+        <v>2</v>
+      </c>
+      <c r="H119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>36</v>
+      </c>
+      <c r="B120">
+        <v>3</v>
+      </c>
+      <c r="C120">
+        <v>5</v>
+      </c>
+      <c r="D120" t="s">
+        <v>27</v>
+      </c>
+      <c r="E120">
+        <v>11.6</v>
+      </c>
+      <c r="F120">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G120">
+        <v>1</v>
+      </c>
+      <c r="H120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>36</v>
+      </c>
+      <c r="B121">
+        <v>3</v>
+      </c>
+      <c r="C121">
+        <v>6</v>
+      </c>
+      <c r="D121" t="s">
+        <v>27</v>
+      </c>
+      <c r="E121">
+        <v>9</v>
+      </c>
+      <c r="F121">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G121">
+        <v>2</v>
+      </c>
+      <c r="H121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>36</v>
+      </c>
+      <c r="B122">
+        <v>3</v>
+      </c>
+      <c r="C122">
+        <v>7</v>
+      </c>
+      <c r="D122" t="s">
+        <v>33</v>
+      </c>
+      <c r="E122">
+        <v>9.5</v>
+      </c>
+      <c r="F122">
+        <v>7.2</v>
+      </c>
+      <c r="G122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>36</v>
+      </c>
+      <c r="B123">
+        <v>3</v>
+      </c>
+      <c r="C123">
+        <v>8</v>
+      </c>
+      <c r="D123" t="s">
+        <v>33</v>
+      </c>
+      <c r="E123">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F123">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G123">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>36</v>
+      </c>
+      <c r="B124">
+        <v>3</v>
+      </c>
+      <c r="C124">
+        <v>9</v>
+      </c>
+      <c r="D124" t="s">
+        <v>37</v>
+      </c>
+      <c r="E124">
+        <v>4.3</v>
+      </c>
+      <c r="F124">
+        <v>6</v>
+      </c>
+      <c r="G124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>36</v>
+      </c>
+      <c r="B125">
+        <v>3</v>
+      </c>
+      <c r="C125">
+        <v>10</v>
+      </c>
+      <c r="D125" t="s">
+        <v>27</v>
+      </c>
+      <c r="E125">
+        <v>7.1</v>
+      </c>
+      <c r="F125">
+        <v>7</v>
+      </c>
+      <c r="G125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>36</v>
+      </c>
+      <c r="B126">
+        <v>3</v>
+      </c>
+      <c r="C126">
+        <v>11</v>
+      </c>
+      <c r="D126" t="s">
+        <v>29</v>
+      </c>
+      <c r="E126">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F126">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G126">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>36</v>
+      </c>
+      <c r="B127">
+        <v>4</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127" t="s">
+        <v>27</v>
+      </c>
+      <c r="E127">
+        <v>13.3</v>
+      </c>
+      <c r="F127">
+        <v>9.5</v>
+      </c>
+      <c r="G127">
+        <v>2</v>
+      </c>
+      <c r="H127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>36</v>
+      </c>
+      <c r="B128">
+        <v>4</v>
+      </c>
+      <c r="C128">
+        <v>2</v>
+      </c>
+      <c r="D128" t="s">
+        <v>28</v>
+      </c>
+      <c r="E128">
+        <v>9.6</v>
+      </c>
+      <c r="F128">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G128">
+        <v>2</v>
+      </c>
+      <c r="H128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>36</v>
+      </c>
+      <c r="B129">
+        <v>4</v>
+      </c>
+      <c r="C129">
+        <v>3</v>
+      </c>
+      <c r="D129" t="s">
+        <v>27</v>
+      </c>
+      <c r="E129">
+        <v>9.5</v>
+      </c>
+      <c r="F129">
+        <v>8.9</v>
+      </c>
+      <c r="G129">
+        <v>2</v>
+      </c>
+      <c r="H129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>36</v>
+      </c>
+      <c r="B130">
+        <v>4</v>
+      </c>
+      <c r="C130">
+        <v>4</v>
+      </c>
+      <c r="D130" t="s">
+        <v>27</v>
+      </c>
+      <c r="E130">
+        <v>12.5</v>
+      </c>
+      <c r="F130">
+        <v>10.9</v>
+      </c>
+      <c r="G130">
+        <v>2</v>
+      </c>
+      <c r="H130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>36</v>
+      </c>
+      <c r="B131">
+        <v>4</v>
+      </c>
+      <c r="C131">
+        <v>5</v>
+      </c>
+      <c r="D131" t="s">
+        <v>28</v>
+      </c>
+      <c r="E131">
+        <v>8</v>
+      </c>
+      <c r="F131">
+        <v>7.6</v>
+      </c>
+      <c r="G131">
+        <v>2</v>
+      </c>
+      <c r="H131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>36</v>
+      </c>
+      <c r="B132">
+        <v>4</v>
+      </c>
+      <c r="C132">
+        <v>6</v>
+      </c>
+      <c r="D132" t="s">
+        <v>26</v>
+      </c>
+      <c r="E132">
+        <v>5</v>
+      </c>
+      <c r="F132">
+        <v>5.4</v>
+      </c>
+      <c r="G132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>36</v>
+      </c>
+      <c r="B133">
+        <v>4</v>
+      </c>
+      <c r="C133">
+        <v>7</v>
+      </c>
+      <c r="D133" t="s">
+        <v>33</v>
+      </c>
+      <c r="E133">
+        <v>6.9</v>
+      </c>
+      <c r="F133">
+        <v>7.4</v>
+      </c>
+      <c r="G133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>36</v>
+      </c>
+      <c r="B134">
+        <v>4</v>
+      </c>
+      <c r="C134">
+        <v>8</v>
+      </c>
+      <c r="D134" t="s">
+        <v>27</v>
+      </c>
+      <c r="E134">
+        <v>7.2</v>
+      </c>
+      <c r="F134">
+        <v>6.2</v>
+      </c>
+      <c r="G134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>36</v>
+      </c>
+      <c r="B135">
+        <v>4</v>
+      </c>
+      <c r="C135">
+        <v>9</v>
+      </c>
+      <c r="D135" t="s">
+        <v>28</v>
+      </c>
+      <c r="E135">
+        <v>5.9</v>
+      </c>
+      <c r="F135">
+        <v>6.7</v>
+      </c>
+      <c r="G135">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>36</v>
+      </c>
+      <c r="B136">
+        <v>4</v>
+      </c>
+      <c r="C136">
+        <v>10</v>
+      </c>
+      <c r="D136" t="s">
+        <v>26</v>
+      </c>
+      <c r="E136">
+        <v>7.3</v>
+      </c>
+      <c r="F136">
+        <v>8.4</v>
+      </c>
+      <c r="G136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>36</v>
+      </c>
+      <c r="B137">
+        <v>5</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+      <c r="D137" t="s">
+        <v>28</v>
+      </c>
+      <c r="E137">
+        <v>10.5</v>
+      </c>
+      <c r="F137">
+        <v>9</v>
+      </c>
+      <c r="G137">
+        <v>2</v>
+      </c>
+      <c r="H137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>36</v>
+      </c>
+      <c r="B138">
+        <v>5</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+      <c r="D138" t="s">
+        <v>28</v>
+      </c>
+      <c r="E138">
+        <v>13.8</v>
+      </c>
+      <c r="F138">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G138">
+        <v>2</v>
+      </c>
+      <c r="H138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>36</v>
+      </c>
+      <c r="B139">
+        <v>5</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
+      </c>
+      <c r="D139" t="s">
+        <v>28</v>
+      </c>
+      <c r="E139">
+        <v>10.7</v>
+      </c>
+      <c r="F139">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G139">
+        <v>2</v>
+      </c>
+      <c r="H139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>36</v>
+      </c>
+      <c r="B140">
+        <v>5</v>
+      </c>
+      <c r="C140">
+        <v>4</v>
+      </c>
+      <c r="D140" t="s">
+        <v>29</v>
+      </c>
+      <c r="E140">
+        <v>5.6</v>
+      </c>
+      <c r="F140">
+        <v>5.3</v>
+      </c>
+      <c r="G140">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>36</v>
+      </c>
+      <c r="B141">
+        <v>5</v>
+      </c>
+      <c r="C141">
+        <v>5</v>
+      </c>
+      <c r="D141" t="s">
+        <v>26</v>
+      </c>
+      <c r="E141">
+        <v>6.1</v>
+      </c>
+      <c r="F141">
+        <v>6.6</v>
+      </c>
+      <c r="G141">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>36</v>
+      </c>
+      <c r="B142">
+        <v>5</v>
+      </c>
+      <c r="C142">
+        <v>6</v>
+      </c>
+      <c r="D142" t="s">
+        <v>26</v>
+      </c>
+      <c r="E142">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F142">
+        <v>5.8</v>
+      </c>
+      <c r="G142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>36</v>
+      </c>
+      <c r="B143">
+        <v>5</v>
+      </c>
+      <c r="C143">
+        <v>7</v>
+      </c>
+      <c r="D143" t="s">
+        <v>29</v>
+      </c>
+      <c r="E143">
+        <v>5.5</v>
+      </c>
+      <c r="F143">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G143">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>36</v>
+      </c>
+      <c r="B144">
+        <v>5</v>
+      </c>
+      <c r="C144">
+        <v>8</v>
+      </c>
+      <c r="D144" t="s">
+        <v>26</v>
+      </c>
+      <c r="E144">
+        <v>4.8</v>
+      </c>
+      <c r="F144">
+        <v>6.9</v>
+      </c>
+      <c r="G144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>36</v>
+      </c>
+      <c r="B145">
+        <v>5</v>
+      </c>
+      <c r="C145">
+        <v>9</v>
+      </c>
+      <c r="D145" t="s">
+        <v>26</v>
+      </c>
+      <c r="E145">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F145">
+        <v>6.1</v>
+      </c>
+      <c r="G145">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>36</v>
+      </c>
+      <c r="B146">
+        <v>5</v>
+      </c>
+      <c r="C146">
+        <v>10</v>
+      </c>
+      <c r="D146" t="s">
+        <v>26</v>
+      </c>
+      <c r="E146">
+        <v>5.4</v>
+      </c>
+      <c r="F146">
+        <v>7.7</v>
+      </c>
+      <c r="G146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>36</v>
+      </c>
+      <c r="B147">
+        <v>5</v>
+      </c>
+      <c r="C147">
+        <v>11</v>
+      </c>
+      <c r="D147" t="s">
+        <v>29</v>
+      </c>
+      <c r="E147">
+        <v>6.1</v>
+      </c>
+      <c r="F147">
+        <v>5.8</v>
+      </c>
+      <c r="G147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>36</v>
+      </c>
+      <c r="B148">
+        <v>6</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+      <c r="D148" t="s">
+        <v>28</v>
+      </c>
+      <c r="E148">
+        <v>11.6</v>
+      </c>
+      <c r="F148">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G148">
+        <v>2</v>
+      </c>
+      <c r="H148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>36</v>
+      </c>
+      <c r="B149">
+        <v>6</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
+      </c>
+      <c r="D149" t="s">
+        <v>28</v>
+      </c>
+      <c r="E149">
+        <v>9</v>
+      </c>
+      <c r="F149">
+        <v>7.3</v>
+      </c>
+      <c r="G149">
+        <v>2</v>
+      </c>
+      <c r="H149">
+        <v>1</v>
+      </c>
+      <c r="L149" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>36</v>
+      </c>
+      <c r="B150">
+        <v>6</v>
+      </c>
+      <c r="C150">
+        <v>3</v>
+      </c>
+      <c r="D150" t="s">
+        <v>28</v>
+      </c>
+      <c r="E150">
+        <v>12.1</v>
+      </c>
+      <c r="F150">
+        <v>7.6</v>
+      </c>
+      <c r="G150">
+        <v>2</v>
+      </c>
+      <c r="H150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>36</v>
+      </c>
+      <c r="B151">
+        <v>6</v>
+      </c>
+      <c r="C151">
+        <v>4</v>
+      </c>
+      <c r="D151" t="s">
+        <v>33</v>
+      </c>
+      <c r="E151">
+        <v>4.5</v>
+      </c>
+      <c r="F151">
+        <v>3.9</v>
+      </c>
+      <c r="G151">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>36</v>
+      </c>
+      <c r="B152">
+        <v>7</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152" t="s">
+        <v>27</v>
+      </c>
+      <c r="E152">
+        <v>14.9</v>
+      </c>
+      <c r="F152">
+        <v>12.8</v>
+      </c>
+      <c r="G152">
+        <v>2</v>
+      </c>
+      <c r="H152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>36</v>
+      </c>
+      <c r="B153">
+        <v>7</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+      <c r="D153" t="s">
+        <v>27</v>
+      </c>
+      <c r="E153">
+        <v>12</v>
+      </c>
+      <c r="F153">
+        <v>11.2</v>
+      </c>
+      <c r="G153">
+        <v>2</v>
+      </c>
+      <c r="H153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>36</v>
+      </c>
+      <c r="B154">
+        <v>7</v>
+      </c>
+      <c r="C154">
+        <v>3</v>
+      </c>
+      <c r="D154" t="s">
+        <v>27</v>
+      </c>
+      <c r="E154">
+        <v>17</v>
+      </c>
+      <c r="F154">
+        <v>13.3</v>
+      </c>
+      <c r="G154">
+        <v>2</v>
+      </c>
+      <c r="H154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>36</v>
+      </c>
+      <c r="B155">
+        <v>7</v>
+      </c>
+      <c r="C155">
+        <v>4</v>
+      </c>
+      <c r="D155" t="s">
+        <v>27</v>
+      </c>
+      <c r="E155">
+        <v>17.3</v>
+      </c>
+      <c r="F155">
+        <v>13.3</v>
+      </c>
+      <c r="G155">
+        <v>2</v>
+      </c>
+      <c r="H155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>36</v>
+      </c>
+      <c r="B156">
+        <v>7</v>
+      </c>
+      <c r="C156">
+        <v>5</v>
+      </c>
+      <c r="D156" t="s">
+        <v>27</v>
+      </c>
+      <c r="E156">
+        <v>17</v>
+      </c>
+      <c r="F156">
+        <v>12.6</v>
+      </c>
+      <c r="G156">
+        <v>2</v>
+      </c>
+      <c r="H156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>36</v>
+      </c>
+      <c r="B157">
+        <v>7</v>
+      </c>
+      <c r="C157">
+        <v>6</v>
+      </c>
+      <c r="D157" t="s">
+        <v>28</v>
+      </c>
+      <c r="E157">
+        <v>7.7</v>
+      </c>
+      <c r="F157">
+        <v>9.6</v>
+      </c>
+      <c r="G157">
+        <v>2</v>
+      </c>
+      <c r="H157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>36</v>
+      </c>
+      <c r="B158">
+        <v>7</v>
+      </c>
+      <c r="C158">
+        <v>7</v>
+      </c>
+      <c r="D158" t="s">
+        <v>27</v>
+      </c>
+      <c r="E158">
+        <v>10.7</v>
+      </c>
+      <c r="F158">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>36</v>
+      </c>
+      <c r="B159">
+        <v>7</v>
+      </c>
+      <c r="C159">
+        <v>8</v>
+      </c>
+      <c r="D159" t="s">
+        <v>26</v>
+      </c>
+      <c r="E159">
+        <v>4</v>
+      </c>
+      <c r="F159">
+        <v>6.9</v>
+      </c>
+      <c r="G159">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>36</v>
+      </c>
+      <c r="B160">
+        <v>7</v>
+      </c>
+      <c r="C160">
+        <v>9</v>
+      </c>
+      <c r="D160" t="s">
+        <v>29</v>
+      </c>
+      <c r="E160">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F160">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G160">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>36</v>
+      </c>
+      <c r="B161">
+        <v>7</v>
+      </c>
+      <c r="C161">
+        <v>10</v>
+      </c>
+      <c r="D161" t="s">
+        <v>26</v>
+      </c>
+      <c r="E161">
+        <v>4.7</v>
+      </c>
+      <c r="F161">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>36</v>
+      </c>
+      <c r="B162">
+        <v>7</v>
+      </c>
+      <c r="C162">
+        <v>11</v>
+      </c>
+      <c r="D162" t="s">
+        <v>26</v>
+      </c>
+      <c r="E162">
+        <v>5</v>
+      </c>
+      <c r="F162">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G162">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>36</v>
+      </c>
+      <c r="B163">
+        <v>7</v>
+      </c>
+      <c r="C163">
+        <v>12</v>
+      </c>
+      <c r="D163" t="s">
+        <v>26</v>
+      </c>
+      <c r="E163">
+        <v>4</v>
+      </c>
+      <c r="F163">
+        <v>7.5</v>
+      </c>
+      <c r="G163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>36</v>
+      </c>
+      <c r="B164">
+        <v>8</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+      <c r="D164" t="s">
+        <v>27</v>
+      </c>
+      <c r="E164">
+        <v>12.4</v>
+      </c>
+      <c r="F164">
+        <v>10.7</v>
+      </c>
+      <c r="G164">
+        <v>2</v>
+      </c>
+      <c r="H164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>36</v>
+      </c>
+      <c r="B165">
+        <v>8</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+      <c r="D165" t="s">
+        <v>28</v>
+      </c>
+      <c r="E165">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="F165">
+        <v>11.8</v>
+      </c>
+      <c r="G165">
+        <v>2</v>
+      </c>
+      <c r="H165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>36</v>
+      </c>
+      <c r="B166">
+        <v>8</v>
+      </c>
+      <c r="C166">
+        <v>3</v>
+      </c>
+      <c r="D166" t="s">
+        <v>27</v>
+      </c>
+      <c r="E166">
+        <v>5.9</v>
+      </c>
+      <c r="F166">
+        <v>6.8</v>
+      </c>
+      <c r="G166">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>36</v>
+      </c>
+      <c r="B167">
+        <v>8</v>
+      </c>
+      <c r="C167">
+        <v>4</v>
+      </c>
+      <c r="D167" t="s">
+        <v>27</v>
+      </c>
+      <c r="E167">
+        <v>4.8</v>
+      </c>
+      <c r="F167">
+        <v>5.5</v>
+      </c>
+      <c r="G167">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>36</v>
+      </c>
+      <c r="B168">
+        <v>8</v>
+      </c>
+      <c r="C168">
+        <v>5</v>
+      </c>
+      <c r="D168" t="s">
+        <v>27</v>
+      </c>
+      <c r="E168">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F168">
+        <v>8.4</v>
+      </c>
+      <c r="G168">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>36</v>
+      </c>
+      <c r="B169">
+        <v>8</v>
+      </c>
+      <c r="C169">
+        <v>6</v>
+      </c>
+      <c r="D169" t="s">
+        <v>26</v>
+      </c>
+      <c r="E169">
+        <v>6</v>
+      </c>
+      <c r="F169">
+        <v>7.1</v>
+      </c>
+      <c r="G169">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>36</v>
+      </c>
+      <c r="B170">
+        <v>8</v>
+      </c>
+      <c r="C170">
+        <v>7</v>
+      </c>
+      <c r="D170" t="s">
+        <v>39</v>
+      </c>
+      <c r="E170">
+        <v>5.9</v>
+      </c>
+      <c r="F170">
+        <v>4.7</v>
+      </c>
+      <c r="G170">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>36</v>
+      </c>
+      <c r="B171">
+        <v>8</v>
+      </c>
+      <c r="C171">
+        <v>8</v>
+      </c>
+      <c r="D171" t="s">
+        <v>26</v>
+      </c>
+      <c r="E171">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F171">
+        <v>5.7</v>
+      </c>
+      <c r="G171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>36</v>
+      </c>
+      <c r="B172">
+        <v>8</v>
+      </c>
+      <c r="C172">
+        <v>9</v>
+      </c>
+      <c r="D172" t="s">
+        <v>27</v>
+      </c>
+      <c r="E172">
+        <v>8.5</v>
+      </c>
+      <c r="F172">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G172">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>36</v>
+      </c>
+      <c r="B173">
+        <v>8</v>
+      </c>
+      <c r="C173">
+        <v>10</v>
+      </c>
+      <c r="D173" t="s">
+        <v>29</v>
+      </c>
+      <c r="E173">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F173">
+        <v>4.8</v>
+      </c>
+      <c r="G173">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>36</v>
+      </c>
+      <c r="B174">
+        <v>8</v>
+      </c>
+      <c r="C174">
+        <v>11</v>
+      </c>
+      <c r="D174" t="s">
+        <v>29</v>
+      </c>
+      <c r="E174">
+        <v>5.2</v>
+      </c>
+      <c r="F174">
+        <v>4</v>
+      </c>
+      <c r="G174">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>36</v>
+      </c>
+      <c r="B175">
+        <v>8</v>
+      </c>
+      <c r="C175">
+        <v>12</v>
+      </c>
+      <c r="D175" t="s">
+        <v>39</v>
+      </c>
+      <c r="E175">
+        <v>4.7</v>
+      </c>
+      <c r="F175">
+        <v>4.7</v>
+      </c>
+      <c r="G175">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>